<commit_message>
Added a file for analysis
</commit_message>
<xml_diff>
--- a/Subjects/Информатика.xlsx
+++ b/Subjects/Информатика.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipluk\PycharmProjects\Курсач\Subjects\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471F3AA5-D398-4DC8-8495-09432C1E57A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2688" yWindow="1140" windowWidth="16248" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -6898,8 +6904,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6958,17 +6964,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7006,9 +7020,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7040,9 +7054,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7074,9 +7106,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7249,14 +7299,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BMZ332"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1716">
+    <row r="1" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12406,7 +12458,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="2" spans="1:1716">
+    <row r="2" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1716</v>
       </c>
@@ -12489,7 +12541,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="3" spans="1:1716">
+    <row r="3" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1717</v>
       </c>
@@ -12560,7 +12612,7 @@
         <v>2123</v>
       </c>
     </row>
-    <row r="4" spans="1:1716">
+    <row r="4" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1718</v>
       </c>
@@ -12643,7 +12695,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="5" spans="1:1716">
+    <row r="5" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1719</v>
       </c>
@@ -12699,7 +12751,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="6" spans="1:1716">
+    <row r="6" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1720</v>
       </c>
@@ -12767,7 +12819,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="7" spans="1:1716">
+    <row r="7" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1721</v>
       </c>
@@ -12886,7 +12938,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="8" spans="1:1716">
+    <row r="8" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1722</v>
       </c>
@@ -12948,7 +13000,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="9" spans="1:1716">
+    <row r="9" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1723</v>
       </c>
@@ -13001,7 +13053,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="10" spans="1:1716">
+    <row r="10" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1724</v>
       </c>
@@ -13066,7 +13118,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="11" spans="1:1716">
+    <row r="11" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1725</v>
       </c>
@@ -13590,7 +13642,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="12" spans="1:1716">
+    <row r="12" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1726</v>
       </c>
@@ -14144,7 +14196,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="13" spans="1:1716">
+    <row r="13" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1727</v>
       </c>
@@ -14260,7 +14312,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="14" spans="1:1716">
+    <row r="14" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1728</v>
       </c>
@@ -14358,7 +14410,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="15" spans="1:1716">
+    <row r="15" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1729</v>
       </c>
@@ -14411,7 +14463,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="16" spans="1:1716">
+    <row r="16" spans="1:1716" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1730</v>
       </c>
@@ -14728,7 +14780,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="17" spans="1:487">
+    <row r="17" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1731</v>
       </c>
@@ -14859,7 +14911,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="18" spans="1:487">
+    <row r="18" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1732</v>
       </c>
@@ -14978,7 +15030,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="19" spans="1:487">
+    <row r="19" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1733</v>
       </c>
@@ -15031,7 +15083,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="20" spans="1:487">
+    <row r="20" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1734</v>
       </c>
@@ -15126,7 +15178,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="21" spans="1:487">
+    <row r="21" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1735</v>
       </c>
@@ -15176,7 +15228,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="22" spans="1:487">
+    <row r="22" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1736</v>
       </c>
@@ -15238,7 +15290,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="23" spans="1:487">
+    <row r="23" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1737</v>
       </c>
@@ -15318,7 +15370,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="24" spans="1:487">
+    <row r="24" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1738</v>
       </c>
@@ -15431,7 +15483,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="25" spans="1:487">
+    <row r="25" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1739</v>
       </c>
@@ -15469,7 +15521,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="26" spans="1:487">
+    <row r="26" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1740</v>
       </c>
@@ -15576,7 +15628,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="27" spans="1:487">
+    <row r="27" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1741</v>
       </c>
@@ -15731,7 +15783,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="28" spans="1:487">
+    <row r="28" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1742</v>
       </c>
@@ -15811,7 +15863,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="29" spans="1:487">
+    <row r="29" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1743</v>
       </c>
@@ -15906,7 +15958,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="30" spans="1:487">
+    <row r="30" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1744</v>
       </c>
@@ -16070,7 +16122,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="31" spans="1:487">
+    <row r="31" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1745</v>
       </c>
@@ -16126,7 +16178,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="32" spans="1:487">
+    <row r="32" spans="1:487" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1746</v>
       </c>
@@ -16179,7 +16231,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="33" spans="1:592">
+    <row r="33" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1747</v>
       </c>
@@ -16256,7 +16308,7 @@
         <v>2165</v>
       </c>
     </row>
-    <row r="34" spans="1:592">
+    <row r="34" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1748</v>
       </c>
@@ -16348,7 +16400,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="35" spans="1:592">
+    <row r="35" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1749</v>
       </c>
@@ -16464,7 +16516,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="36" spans="1:592">
+    <row r="36" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1750</v>
       </c>
@@ -16553,7 +16605,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="37" spans="1:592">
+    <row r="37" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1751</v>
       </c>
@@ -16597,7 +16649,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="38" spans="1:592">
+    <row r="38" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1752</v>
       </c>
@@ -16671,7 +16723,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="39" spans="1:592">
+    <row r="39" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1753</v>
       </c>
@@ -16766,7 +16818,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="40" spans="1:592">
+    <row r="40" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1754</v>
       </c>
@@ -16813,7 +16865,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="41" spans="1:592">
+    <row r="41" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1755</v>
       </c>
@@ -16878,7 +16930,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="42" spans="1:592">
+    <row r="42" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1756</v>
       </c>
@@ -16940,7 +16992,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="43" spans="1:592">
+    <row r="43" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1757</v>
       </c>
@@ -17050,7 +17102,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="44" spans="1:592">
+    <row r="44" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1758</v>
       </c>
@@ -17178,7 +17230,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="45" spans="1:592">
+    <row r="45" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1759</v>
       </c>
@@ -17255,7 +17307,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="46" spans="1:592">
+    <row r="46" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1760</v>
       </c>
@@ -17323,7 +17375,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="47" spans="1:592">
+    <row r="47" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1761</v>
       </c>
@@ -17538,7 +17590,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="48" spans="1:592">
+    <row r="48" spans="1:592" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1762</v>
       </c>
@@ -17678,7 +17730,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="49" spans="1:793">
+    <row r="49" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>1763</v>
       </c>
@@ -17779,7 +17831,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="50" spans="1:793">
+    <row r="50" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1764</v>
       </c>
@@ -17829,7 +17881,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="51" spans="1:793">
+    <row r="51" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>1765</v>
       </c>
@@ -17891,7 +17943,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="52" spans="1:793">
+    <row r="52" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>1766</v>
       </c>
@@ -18034,7 +18086,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="53" spans="1:793">
+    <row r="53" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1767</v>
       </c>
@@ -18072,7 +18124,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="54" spans="1:793">
+    <row r="54" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1768</v>
       </c>
@@ -18263,7 +18315,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="55" spans="1:793">
+    <row r="55" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>1769</v>
       </c>
@@ -18310,7 +18362,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="56" spans="1:793">
+    <row r="56" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>1770</v>
       </c>
@@ -18405,7 +18457,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="57" spans="1:793">
+    <row r="57" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>1771</v>
       </c>
@@ -18878,7 +18930,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="58" spans="1:793">
+    <row r="58" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>1772</v>
       </c>
@@ -18916,7 +18968,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="59" spans="1:793">
+    <row r="59" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>1773</v>
       </c>
@@ -19044,7 +19096,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="60" spans="1:793">
+    <row r="60" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>1774</v>
       </c>
@@ -19220,7 +19272,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="61" spans="1:793">
+    <row r="61" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>1775</v>
       </c>
@@ -19279,7 +19331,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="62" spans="1:793">
+    <row r="62" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>1776</v>
       </c>
@@ -19581,7 +19633,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="63" spans="1:793">
+    <row r="63" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>1777</v>
       </c>
@@ -19688,7 +19740,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="64" spans="1:793">
+    <row r="64" spans="1:793" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>1778</v>
       </c>
@@ -19837,7 +19889,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="65" spans="1:871">
+    <row r="65" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1779</v>
       </c>
@@ -19896,7 +19948,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="66" spans="1:871">
+    <row r="66" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1780</v>
       </c>
@@ -20003,7 +20055,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="67" spans="1:871">
+    <row r="67" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1781</v>
       </c>
@@ -20047,7 +20099,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="68" spans="1:871">
+    <row r="68" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1782</v>
       </c>
@@ -20085,7 +20137,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="69" spans="1:871">
+    <row r="69" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1783</v>
       </c>
@@ -20219,7 +20271,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="70" spans="1:871">
+    <row r="70" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>1784</v>
       </c>
@@ -20293,7 +20345,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="71" spans="1:871">
+    <row r="71" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>1785</v>
       </c>
@@ -20349,7 +20401,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="72" spans="1:871">
+    <row r="72" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>1786</v>
       </c>
@@ -20390,7 +20442,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="73" spans="1:871">
+    <row r="73" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>1787</v>
       </c>
@@ -20461,7 +20513,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="74" spans="1:871">
+    <row r="74" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>1788</v>
       </c>
@@ -20679,7 +20731,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="75" spans="1:871">
+    <row r="75" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>1789</v>
       </c>
@@ -20996,7 +21048,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="76" spans="1:871">
+    <row r="76" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>1790</v>
       </c>
@@ -21040,7 +21092,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="77" spans="1:871">
+    <row r="77" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>1791</v>
       </c>
@@ -21138,7 +21190,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="78" spans="1:871">
+    <row r="78" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>1792</v>
       </c>
@@ -21194,7 +21246,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="79" spans="1:871">
+    <row r="79" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1793</v>
       </c>
@@ -21286,7 +21338,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="80" spans="1:871">
+    <row r="80" spans="1:871" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>1794</v>
       </c>
@@ -21363,7 +21415,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="81" spans="1:1037">
+    <row r="81" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>1795</v>
       </c>
@@ -21587,7 +21639,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="82" spans="1:1037">
+    <row r="82" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>1796</v>
       </c>
@@ -21655,7 +21707,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="83" spans="1:1037">
+    <row r="83" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>1797</v>
       </c>
@@ -21708,7 +21760,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="84" spans="1:1037">
+    <row r="84" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>1798</v>
       </c>
@@ -21803,7 +21855,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="85" spans="1:1037">
+    <row r="85" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>1799</v>
       </c>
@@ -22381,7 +22433,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="86" spans="1:1037">
+    <row r="86" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>1800</v>
       </c>
@@ -22479,7 +22531,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="87" spans="1:1037">
+    <row r="87" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>1801</v>
       </c>
@@ -22520,7 +22572,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="88" spans="1:1037">
+    <row r="88" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>1802</v>
       </c>
@@ -22837,7 +22889,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="89" spans="1:1037">
+    <row r="89" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>1803</v>
       </c>
@@ -22884,7 +22936,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="90" spans="1:1037">
+    <row r="90" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>1804</v>
       </c>
@@ -22946,7 +22998,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="91" spans="1:1037">
+    <row r="91" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>1805</v>
       </c>
@@ -23008,7 +23060,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="92" spans="1:1037">
+    <row r="92" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>1806</v>
       </c>
@@ -23154,7 +23206,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="93" spans="1:1037">
+    <row r="93" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>1807</v>
       </c>
@@ -23258,7 +23310,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="94" spans="1:1037">
+    <row r="94" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>1808</v>
       </c>
@@ -23320,7 +23372,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="95" spans="1:1037">
+    <row r="95" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>1809</v>
       </c>
@@ -23415,7 +23467,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="96" spans="1:1037">
+    <row r="96" spans="1:1037" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>1810</v>
       </c>
@@ -23459,7 +23511,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="97" spans="1:1125">
+    <row r="97" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>1811</v>
       </c>
@@ -23593,7 +23645,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="98" spans="1:1125">
+    <row r="98" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>1812</v>
       </c>
@@ -23733,7 +23785,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="99" spans="1:1125">
+    <row r="99" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>1813</v>
       </c>
@@ -23867,7 +23919,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="100" spans="1:1125">
+    <row r="100" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>1814</v>
       </c>
@@ -23914,7 +23966,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="101" spans="1:1125">
+    <row r="101" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>1815</v>
       </c>
@@ -23991,7 +24043,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="102" spans="1:1125">
+    <row r="102" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>1816</v>
       </c>
@@ -24029,7 +24081,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="103" spans="1:1125">
+    <row r="103" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>1817</v>
       </c>
@@ -24100,7 +24152,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="104" spans="1:1125">
+    <row r="104" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>1818</v>
       </c>
@@ -24135,7 +24187,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="105" spans="1:1125">
+    <row r="105" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>1819</v>
       </c>
@@ -24206,7 +24258,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="106" spans="1:1125">
+    <row r="106" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>1820</v>
       </c>
@@ -24283,7 +24335,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="107" spans="1:1125">
+    <row r="107" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>1821</v>
       </c>
@@ -24423,7 +24475,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="108" spans="1:1125">
+    <row r="108" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>1822</v>
       </c>
@@ -24671,7 +24723,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="109" spans="1:1125">
+    <row r="109" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>1823</v>
       </c>
@@ -24790,7 +24842,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="110" spans="1:1125">
+    <row r="110" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>1824</v>
       </c>
@@ -24915,7 +24967,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="111" spans="1:1125">
+    <row r="111" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>1825</v>
       </c>
@@ -24962,7 +25014,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="112" spans="1:1125">
+    <row r="112" spans="1:892 1038:1125" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>1826</v>
       </c>
@@ -25033,7 +25085,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="113" spans="1:1181">
+    <row r="113" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>1827</v>
       </c>
@@ -25098,7 +25150,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="114" spans="1:1181">
+    <row r="114" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>1828</v>
       </c>
@@ -25142,7 +25194,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="115" spans="1:1181">
+    <row r="115" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>1829</v>
       </c>
@@ -25204,7 +25256,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="116" spans="1:1181">
+    <row r="116" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>1830</v>
       </c>
@@ -25332,7 +25384,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="117" spans="1:1181">
+    <row r="117" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>1831</v>
       </c>
@@ -25379,7 +25431,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="118" spans="1:1181">
+    <row r="118" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>1832</v>
       </c>
@@ -25585,7 +25637,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="119" spans="1:1181">
+    <row r="119" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>1833</v>
       </c>
@@ -25728,7 +25780,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="120" spans="1:1181">
+    <row r="120" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>1834</v>
       </c>
@@ -25787,7 +25839,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="121" spans="1:1181">
+    <row r="121" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>1835</v>
       </c>
@@ -25858,7 +25910,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="122" spans="1:1181">
+    <row r="122" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>1836</v>
       </c>
@@ -25899,7 +25951,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="123" spans="1:1181">
+    <row r="123" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>1837</v>
       </c>
@@ -25940,7 +25992,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="124" spans="1:1181">
+    <row r="124" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>1838</v>
       </c>
@@ -26038,7 +26090,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="125" spans="1:1181">
+    <row r="125" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>1839</v>
       </c>
@@ -26091,7 +26143,7 @@
         <v>2152</v>
       </c>
     </row>
-    <row r="126" spans="1:1181">
+    <row r="126" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>1840</v>
       </c>
@@ -26177,7 +26229,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="127" spans="1:1181">
+    <row r="127" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>1841</v>
       </c>
@@ -26218,7 +26270,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="128" spans="1:1181">
+    <row r="128" spans="1:913 1048:1181" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>1842</v>
       </c>
@@ -26286,7 +26338,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="129" spans="1:1249">
+    <row r="129" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>1843</v>
       </c>
@@ -26504,7 +26556,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="130" spans="1:1249">
+    <row r="130" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>1844</v>
       </c>
@@ -26572,7 +26624,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="131" spans="1:1249">
+    <row r="131" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>1845</v>
       </c>
@@ -26613,7 +26665,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="132" spans="1:1249">
+    <row r="132" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>1846</v>
       </c>
@@ -26687,7 +26739,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="133" spans="1:1249">
+    <row r="133" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>1847</v>
       </c>
@@ -26728,7 +26780,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="134" spans="1:1249">
+    <row r="134" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>1848</v>
       </c>
@@ -26757,7 +26809,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="135" spans="1:1249">
+    <row r="135" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>1849</v>
       </c>
@@ -26900,7 +26952,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="136" spans="1:1249">
+    <row r="136" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>1850</v>
       </c>
@@ -27064,7 +27116,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="137" spans="1:1249">
+    <row r="137" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>1851</v>
       </c>
@@ -27126,7 +27178,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="138" spans="1:1249">
+    <row r="138" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>1852</v>
       </c>
@@ -27284,7 +27336,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="139" spans="1:1249">
+    <row r="139" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>1853</v>
       </c>
@@ -27364,7 +27416,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="140" spans="1:1249">
+    <row r="140" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>1854</v>
       </c>
@@ -27396,7 +27448,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="141" spans="1:1249">
+    <row r="141" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>1855</v>
       </c>
@@ -27485,7 +27537,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="142" spans="1:1249">
+    <row r="142" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>1856</v>
       </c>
@@ -27571,7 +27623,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="143" spans="1:1249">
+    <row r="143" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>1857</v>
       </c>
@@ -27714,7 +27766,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="144" spans="1:1249">
+    <row r="144" spans="1:1021 1025:1249" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>1858</v>
       </c>
@@ -27779,7 +27831,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="145" spans="1:1298">
+    <row r="145" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>1859</v>
       </c>
@@ -27814,7 +27866,7 @@
         <v>2148</v>
       </c>
     </row>
-    <row r="146" spans="1:1298">
+    <row r="146" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>1860</v>
       </c>
@@ -27852,7 +27904,7 @@
         <v>2149</v>
       </c>
     </row>
-    <row r="147" spans="1:1298">
+    <row r="147" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>1861</v>
       </c>
@@ -27950,7 +28002,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="148" spans="1:1298">
+    <row r="148" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>1862</v>
       </c>
@@ -27997,7 +28049,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="149" spans="1:1298">
+    <row r="149" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>1863</v>
       </c>
@@ -28086,7 +28138,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="150" spans="1:1298">
+    <row r="150" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>1864</v>
       </c>
@@ -28145,7 +28197,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="151" spans="1:1298">
+    <row r="151" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>1865</v>
       </c>
@@ -28207,7 +28259,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="152" spans="1:1298">
+    <row r="152" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>1866</v>
       </c>
@@ -28233,7 +28285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:1298">
+    <row r="153" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>1867</v>
       </c>
@@ -28265,7 +28317,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="154" spans="1:1298">
+    <row r="154" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>1868</v>
       </c>
@@ -28516,7 +28568,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="155" spans="1:1298">
+    <row r="155" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>1869</v>
       </c>
@@ -28719,7 +28771,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="156" spans="1:1298">
+    <row r="156" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>1870</v>
       </c>
@@ -28754,7 +28806,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="157" spans="1:1298">
+    <row r="157" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>1871</v>
       </c>
@@ -28783,7 +28835,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="158" spans="1:1298">
+    <row r="158" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>1872</v>
       </c>
@@ -28833,7 +28885,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="159" spans="1:1298">
+    <row r="159" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>1873</v>
       </c>
@@ -28892,7 +28944,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="160" spans="1:1298">
+    <row r="160" spans="1:877 1039:1298" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>1874</v>
       </c>
@@ -28921,7 +28973,7 @@
         <v>2148</v>
       </c>
     </row>
-    <row r="161" spans="1:1327">
+    <row r="161" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>1875</v>
       </c>
@@ -28980,7 +29032,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="162" spans="1:1327">
+    <row r="162" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>1876</v>
       </c>
@@ -29183,7 +29235,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="163" spans="1:1327">
+    <row r="163" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>1877</v>
       </c>
@@ -29224,7 +29276,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="164" spans="1:1327">
+    <row r="164" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>1878</v>
       </c>
@@ -29277,7 +29329,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="165" spans="1:1327">
+    <row r="165" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>1879</v>
       </c>
@@ -29381,7 +29433,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="166" spans="1:1327">
+    <row r="166" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>1880</v>
       </c>
@@ -29479,7 +29531,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="167" spans="1:1327">
+    <row r="167" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>1881</v>
       </c>
@@ -29517,7 +29569,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="168" spans="1:1327">
+    <row r="168" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>1882</v>
       </c>
@@ -29738,7 +29790,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="169" spans="1:1327">
+    <row r="169" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>1883</v>
       </c>
@@ -29803,7 +29855,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="170" spans="1:1327">
+    <row r="170" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>1884</v>
       </c>
@@ -29850,7 +29902,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="171" spans="1:1327">
+    <row r="171" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>1885</v>
       </c>
@@ -29960,7 +30012,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="172" spans="1:1327">
+    <row r="172" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>1886</v>
       </c>
@@ -30028,7 +30080,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="173" spans="1:1327">
+    <row r="173" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>1887</v>
       </c>
@@ -30096,7 +30148,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="174" spans="1:1327">
+    <row r="174" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>1888</v>
       </c>
@@ -30134,7 +30186,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="175" spans="1:1327">
+    <row r="175" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>1889</v>
       </c>
@@ -30238,7 +30290,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="176" spans="1:1327">
+    <row r="176" spans="1:840 1032:1327" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>1890</v>
       </c>
@@ -30303,7 +30355,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="177" spans="1:1377">
+    <row r="177" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>1891</v>
       </c>
@@ -30341,7 +30393,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="178" spans="1:1377">
+    <row r="178" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>1892</v>
       </c>
@@ -30424,7 +30476,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="179" spans="1:1377">
+    <row r="179" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>1893</v>
       </c>
@@ -30462,7 +30514,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="180" spans="1:1377">
+    <row r="180" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>1894</v>
       </c>
@@ -30542,7 +30594,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="181" spans="1:1377">
+    <row r="181" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>1895</v>
       </c>
@@ -30571,7 +30623,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="182" spans="1:1377">
+    <row r="182" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>1896</v>
       </c>
@@ -30630,7 +30682,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="183" spans="1:1377">
+    <row r="183" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>1897</v>
       </c>
@@ -30800,7 +30852,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="184" spans="1:1377">
+    <row r="184" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>1898</v>
       </c>
@@ -30841,7 +30893,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="185" spans="1:1377">
+    <row r="185" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>1899</v>
       </c>
@@ -30918,7 +30970,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="186" spans="1:1377">
+    <row r="186" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>1900</v>
       </c>
@@ -30998,7 +31050,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="187" spans="1:1377">
+    <row r="187" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>1901</v>
       </c>
@@ -31105,7 +31157,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="188" spans="1:1377">
+    <row r="188" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>1902</v>
       </c>
@@ -31149,7 +31201,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="189" spans="1:1377">
+    <row r="189" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>1903</v>
       </c>
@@ -31193,7 +31245,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="190" spans="1:1377">
+    <row r="190" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>1904</v>
       </c>
@@ -31255,7 +31307,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="191" spans="1:1377">
+    <row r="191" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>1905</v>
       </c>
@@ -31311,7 +31363,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="192" spans="1:1377">
+    <row r="192" spans="1:916 1039:1377" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>1906</v>
       </c>
@@ -31382,7 +31434,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="193" spans="1:1388">
+    <row r="193" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>1907</v>
       </c>
@@ -31447,7 +31499,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="194" spans="1:1388">
+    <row r="194" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>1908</v>
       </c>
@@ -31485,7 +31537,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="195" spans="1:1388">
+    <row r="195" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>1909</v>
       </c>
@@ -31538,7 +31590,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="196" spans="1:1388">
+    <row r="196" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>1910</v>
       </c>
@@ -31627,7 +31679,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="197" spans="1:1388">
+    <row r="197" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>1911</v>
       </c>
@@ -31677,7 +31729,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="198" spans="1:1388">
+    <row r="198" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>1912</v>
       </c>
@@ -31718,7 +31770,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="199" spans="1:1388">
+    <row r="199" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>1913</v>
       </c>
@@ -31858,7 +31910,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="200" spans="1:1388">
+    <row r="200" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>1914</v>
       </c>
@@ -31911,7 +31963,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="201" spans="1:1388">
+    <row r="201" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>1915</v>
       </c>
@@ -31937,7 +31989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:1388">
+    <row r="202" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>1916</v>
       </c>
@@ -32032,7 +32084,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="203" spans="1:1388">
+    <row r="203" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>1917</v>
       </c>
@@ -32100,7 +32152,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="204" spans="1:1388">
+    <row r="204" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>1918</v>
       </c>
@@ -32132,7 +32184,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="205" spans="1:1388">
+    <row r="205" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>1919</v>
       </c>
@@ -32161,7 +32213,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="206" spans="1:1388">
+    <row r="206" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>1920</v>
       </c>
@@ -32196,7 +32248,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="207" spans="1:1388">
+    <row r="207" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>1921</v>
       </c>
@@ -32225,7 +32277,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="208" spans="1:1388">
+    <row r="208" spans="1:904 1047:1388" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>1922</v>
       </c>
@@ -32257,7 +32309,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="209" spans="1:1432">
+    <row r="209" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>1923</v>
       </c>
@@ -32361,7 +32413,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="210" spans="1:1432">
+    <row r="210" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>1924</v>
       </c>
@@ -32390,7 +32442,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="211" spans="1:1432">
+    <row r="211" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>1925</v>
       </c>
@@ -32500,7 +32552,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="212" spans="1:1432">
+    <row r="212" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>1926</v>
       </c>
@@ -32532,7 +32584,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="213" spans="1:1432">
+    <row r="213" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>1927</v>
       </c>
@@ -32564,7 +32616,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="214" spans="1:1432">
+    <row r="214" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>1928</v>
       </c>
@@ -32596,7 +32648,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="215" spans="1:1432">
+    <row r="215" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>1929</v>
       </c>
@@ -32703,7 +32755,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="216" spans="1:1432">
+    <row r="216" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>1930</v>
       </c>
@@ -32804,7 +32856,7 @@
         <v>2114</v>
       </c>
     </row>
-    <row r="217" spans="1:1432">
+    <row r="217" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>1931</v>
       </c>
@@ -32836,7 +32888,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="218" spans="1:1432">
+    <row r="218" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>1932</v>
       </c>
@@ -32880,7 +32932,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="219" spans="1:1432">
+    <row r="219" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>1933</v>
       </c>
@@ -32936,7 +32988,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="220" spans="1:1432">
+    <row r="220" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>1934</v>
       </c>
@@ -33004,7 +33056,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="221" spans="1:1432">
+    <row r="221" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>1935</v>
       </c>
@@ -33042,7 +33094,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="222" spans="1:1432">
+    <row r="222" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>1936</v>
       </c>
@@ -33095,7 +33147,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="223" spans="1:1432">
+    <row r="223" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>1937</v>
       </c>
@@ -33172,7 +33224,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="224" spans="1:1432">
+    <row r="224" spans="1:926 1025:1432" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>1938</v>
       </c>
@@ -33270,7 +33322,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="225" spans="1:1535">
+    <row r="225" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>1939</v>
       </c>
@@ -33302,7 +33354,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="226" spans="1:1535">
+    <row r="226" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>1940</v>
       </c>
@@ -33358,7 +33410,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="227" spans="1:1535">
+    <row r="227" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>1941</v>
       </c>
@@ -33417,7 +33469,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="228" spans="1:1535">
+    <row r="228" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>1942</v>
       </c>
@@ -33473,7 +33525,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="229" spans="1:1535">
+    <row r="229" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>1943</v>
       </c>
@@ -33523,7 +33575,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="230" spans="1:1535">
+    <row r="230" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>1944</v>
       </c>
@@ -33582,7 +33634,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="231" spans="1:1535">
+    <row r="231" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>1945</v>
       </c>
@@ -33644,7 +33696,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="232" spans="1:1535">
+    <row r="232" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>1946</v>
       </c>
@@ -33724,7 +33776,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="233" spans="1:1535">
+    <row r="233" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>1947</v>
       </c>
@@ -33753,7 +33805,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="234" spans="1:1535">
+    <row r="234" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>1948</v>
       </c>
@@ -33791,7 +33843,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="235" spans="1:1535">
+    <row r="235" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>1949</v>
       </c>
@@ -33823,7 +33875,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="236" spans="1:1535">
+    <row r="236" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>1950</v>
       </c>
@@ -33870,7 +33922,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="237" spans="1:1535">
+    <row r="237" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>1951</v>
       </c>
@@ -33914,7 +33966,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="238" spans="1:1535">
+    <row r="238" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>1952</v>
       </c>
@@ -33949,7 +34001,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="239" spans="1:1535">
+    <row r="239" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>1953</v>
       </c>
@@ -34047,7 +34099,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="240" spans="1:1535">
+    <row r="240" spans="1:1020 1039:1535" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>1954</v>
       </c>
@@ -34481,7 +34533,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="241" spans="1:1606">
+    <row r="241" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>1955</v>
       </c>
@@ -34570,7 +34622,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="242" spans="1:1606">
+    <row r="242" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>1956</v>
       </c>
@@ -34617,7 +34669,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="243" spans="1:1606">
+    <row r="243" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>1957</v>
       </c>
@@ -34952,7 +35004,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="244" spans="1:1606">
+    <row r="244" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>1958</v>
       </c>
@@ -34996,7 +35048,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="245" spans="1:1606">
+    <row r="245" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>1959</v>
       </c>
@@ -35046,7 +35098,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="246" spans="1:1606">
+    <row r="246" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>1960</v>
       </c>
@@ -35162,7 +35214,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="247" spans="1:1606">
+    <row r="247" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>1961</v>
       </c>
@@ -35221,7 +35273,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="248" spans="1:1606">
+    <row r="248" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>1962</v>
       </c>
@@ -35268,7 +35320,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="249" spans="1:1606">
+    <row r="249" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>1963</v>
       </c>
@@ -35354,7 +35406,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="250" spans="1:1606">
+    <row r="250" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>1964</v>
       </c>
@@ -35395,7 +35447,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="251" spans="1:1606">
+    <row r="251" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>1965</v>
       </c>
@@ -35430,7 +35482,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="252" spans="1:1606">
+    <row r="252" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>1966</v>
       </c>
@@ -35507,7 +35559,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="253" spans="1:1606">
+    <row r="253" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>1967</v>
       </c>
@@ -35542,7 +35594,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="254" spans="1:1606">
+    <row r="254" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>1968</v>
       </c>
@@ -35580,7 +35632,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="255" spans="1:1606">
+    <row r="255" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>1969</v>
       </c>
@@ -35630,7 +35682,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="256" spans="1:1606">
+    <row r="256" spans="1:1020 1026:1606" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>1970</v>
       </c>
@@ -35698,7 +35750,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="257" spans="1:1666">
+    <row r="257" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>1971</v>
       </c>
@@ -35889,7 +35941,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="258" spans="1:1666">
+    <row r="258" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>1972</v>
       </c>
@@ -36023,7 +36075,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="259" spans="1:1666">
+    <row r="259" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>1973</v>
       </c>
@@ -36079,7 +36131,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="260" spans="1:1666">
+    <row r="260" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>1974</v>
       </c>
@@ -36339,7 +36391,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="261" spans="1:1666">
+    <row r="261" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>1975</v>
       </c>
@@ -36377,7 +36429,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="262" spans="1:1666">
+    <row r="262" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>1976</v>
       </c>
@@ -36424,7 +36476,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="263" spans="1:1666">
+    <row r="263" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>1977</v>
       </c>
@@ -36450,7 +36502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:1666">
+    <row r="264" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>1978</v>
       </c>
@@ -36485,7 +36537,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="265" spans="1:1666">
+    <row r="265" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>1979</v>
       </c>
@@ -36568,7 +36620,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="266" spans="1:1666">
+    <row r="266" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>1980</v>
       </c>
@@ -36603,7 +36655,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="267" spans="1:1666">
+    <row r="267" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>1981</v>
       </c>
@@ -36680,7 +36732,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="268" spans="1:1666">
+    <row r="268" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>1982</v>
       </c>
@@ -36736,7 +36788,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="269" spans="1:1666">
+    <row r="269" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>1983</v>
       </c>
@@ -36792,7 +36844,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="270" spans="1:1666">
+    <row r="270" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>1984</v>
       </c>
@@ -36878,7 +36930,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="271" spans="1:1666">
+    <row r="271" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>1985</v>
       </c>
@@ -36931,7 +36983,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="272" spans="1:1666">
+    <row r="272" spans="1:899 1060:1666" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>1986</v>
       </c>
@@ -36996,7 +37048,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="273" spans="1:1701">
+    <row r="273" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>1987</v>
       </c>
@@ -37067,7 +37119,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="274" spans="1:1701">
+    <row r="274" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>1988</v>
       </c>
@@ -37261,7 +37313,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="275" spans="1:1701">
+    <row r="275" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>1989</v>
       </c>
@@ -37455,7 +37507,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="276" spans="1:1701">
+    <row r="276" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>1990</v>
       </c>
@@ -37493,7 +37545,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="277" spans="1:1701">
+    <row r="277" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>1991</v>
       </c>
@@ -37585,7 +37637,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="278" spans="1:1701">
+    <row r="278" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>1992</v>
       </c>
@@ -37683,7 +37735,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="279" spans="1:1701">
+    <row r="279" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>1993</v>
       </c>
@@ -37781,7 +37833,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="280" spans="1:1701">
+    <row r="280" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>1994</v>
       </c>
@@ -37843,7 +37895,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="281" spans="1:1701">
+    <row r="281" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>1995</v>
       </c>
@@ -37902,7 +37954,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="282" spans="1:1701">
+    <row r="282" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>1996</v>
       </c>
@@ -37964,7 +38016,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="283" spans="1:1701">
+    <row r="283" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>1997</v>
       </c>
@@ -38122,7 +38174,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="284" spans="1:1701">
+    <row r="284" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>1998</v>
       </c>
@@ -38187,7 +38239,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="285" spans="1:1701">
+    <row r="285" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>1999</v>
       </c>
@@ -38243,7 +38295,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="286" spans="1:1701">
+    <row r="286" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>2000</v>
       </c>
@@ -38281,7 +38333,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="287" spans="1:1701">
+    <row r="287" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>2001</v>
       </c>
@@ -38367,7 +38419,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="288" spans="1:1701">
+    <row r="288" spans="1:1016 1026:1701" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>2002</v>
       </c>
@@ -38417,7 +38469,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="289" spans="1:1709">
+    <row r="289" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>2003</v>
       </c>
@@ -38455,7 +38507,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="290" spans="1:1709">
+    <row r="290" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>2004</v>
       </c>
@@ -38502,7 +38554,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="291" spans="1:1709">
+    <row r="291" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>2005</v>
       </c>
@@ -38531,7 +38583,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="292" spans="1:1709">
+    <row r="292" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>2006</v>
       </c>
@@ -38566,7 +38618,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="293" spans="1:1709">
+    <row r="293" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>2007</v>
       </c>
@@ -38622,7 +38674,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="294" spans="1:1709">
+    <row r="294" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>2008</v>
       </c>
@@ -38885,7 +38937,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="295" spans="1:1709">
+    <row r="295" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>2009</v>
       </c>
@@ -38914,7 +38966,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="296" spans="1:1709">
+    <row r="296" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>2010</v>
       </c>
@@ -38964,7 +39016,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="297" spans="1:1709">
+    <row r="297" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>2011</v>
       </c>
@@ -39014,7 +39066,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="298" spans="1:1709">
+    <row r="298" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>2012</v>
       </c>
@@ -39046,7 +39098,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="299" spans="1:1709">
+    <row r="299" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>2013</v>
       </c>
@@ -39075,7 +39127,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="300" spans="1:1709">
+    <row r="300" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>2014</v>
       </c>
@@ -39179,7 +39231,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="301" spans="1:1709">
+    <row r="301" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>2015</v>
       </c>
@@ -39223,7 +39275,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="302" spans="1:1709">
+    <row r="302" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>2016</v>
       </c>
@@ -39261,7 +39313,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="303" spans="1:1709">
+    <row r="303" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>2017</v>
       </c>
@@ -39308,7 +39360,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="304" spans="1:1709">
+    <row r="304" spans="1:839 1032:1709" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>2018</v>
       </c>
@@ -39346,7 +39398,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="305" spans="1:1713">
+    <row r="305" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>2019</v>
       </c>
@@ -39396,7 +39448,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="306" spans="1:1713">
+    <row r="306" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>2020</v>
       </c>
@@ -39428,7 +39480,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="307" spans="1:1713">
+    <row r="307" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>2021</v>
       </c>
@@ -39526,7 +39578,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="308" spans="1:1713">
+    <row r="308" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>2022</v>
       </c>
@@ -39570,7 +39622,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="309" spans="1:1713">
+    <row r="309" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>2023</v>
       </c>
@@ -39614,7 +39666,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="310" spans="1:1713">
+    <row r="310" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>2024</v>
       </c>
@@ -39652,7 +39704,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="311" spans="1:1713">
+    <row r="311" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>2025</v>
       </c>
@@ -39684,7 +39736,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="312" spans="1:1713">
+    <row r="312" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>2026</v>
       </c>
@@ -39731,7 +39783,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="313" spans="1:1713">
+    <row r="313" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>2027</v>
       </c>
@@ -39772,7 +39824,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="314" spans="1:1713">
+    <row r="314" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>2028</v>
       </c>
@@ -39819,7 +39871,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="315" spans="1:1713">
+    <row r="315" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>2029</v>
       </c>
@@ -39866,7 +39918,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="316" spans="1:1713">
+    <row r="316" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>2030</v>
       </c>
@@ -39916,7 +39968,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="317" spans="1:1713">
+    <row r="317" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>2031</v>
       </c>
@@ -40026,7 +40078,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="318" spans="1:1713">
+    <row r="318" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>2032</v>
       </c>
@@ -40070,7 +40122,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="319" spans="1:1713">
+    <row r="319" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>2033</v>
       </c>
@@ -40111,7 +40163,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="320" spans="1:1713">
+    <row r="320" spans="1:902 1047:1713" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>2034</v>
       </c>
@@ -40143,7 +40195,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="321" spans="1:1716">
+    <row r="321" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>2035</v>
       </c>
@@ -40208,7 +40260,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="322" spans="1:1716">
+    <row r="322" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>2036</v>
       </c>
@@ -40255,7 +40307,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="323" spans="1:1716">
+    <row r="323" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>2037</v>
       </c>
@@ -40299,7 +40351,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="324" spans="1:1716">
+    <row r="324" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>2038</v>
       </c>
@@ -40331,7 +40383,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="325" spans="1:1716">
+    <row r="325" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>2039</v>
       </c>
@@ -40363,7 +40415,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="326" spans="1:1716">
+    <row r="326" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>2040</v>
       </c>
@@ -40392,7 +40444,7 @@
         <v>2165</v>
       </c>
     </row>
-    <row r="327" spans="1:1716">
+    <row r="327" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>2041</v>
       </c>
@@ -40430,7 +40482,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="328" spans="1:1716">
+    <row r="328" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>2042</v>
       </c>
@@ -40459,7 +40511,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="329" spans="1:1716">
+    <row r="329" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>2043</v>
       </c>
@@ -40518,7 +40570,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="330" spans="1:1716">
+    <row r="330" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>2044</v>
       </c>
@@ -40559,7 +40611,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="331" spans="1:1716">
+    <row r="331" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>2045</v>
       </c>
@@ -40642,7 +40694,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="332" spans="1:1716">
+    <row r="332" spans="1:906 1039:1716" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>2046</v>
       </c>

</xml_diff>